<commit_message>
removendo sqls antigos, adicionando novo, arrumando erro do datepicker, alterando mascara de preço e ajustando pagina de projetos/tarefas
</commit_message>
<xml_diff>
--- a/checklist-tarefas-tcc.xlsx
+++ b/checklist-tarefas-tcc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheusborroshirakawa/www/projeto_tcc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheus/www/projeto_tcc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB72F34-9AC2-8F4E-B5EC-21A2189E2B02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0371E3F3-D2B2-0049-8156-C4967D1387E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{A9902BDF-4FA8-4E47-B561-A17E2967AB32}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Criar seeders para projetos com o foreign key dos usuarios</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Separar todas as ideias dos Relatorios</t>
-  </si>
-  <si>
-    <t>Migrar pro Vue.js</t>
   </si>
   <si>
     <t>Escrever todas as rotas do site</t>
@@ -558,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BE640A-07D6-A746-BA45-5FBA6C6C9BB6}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,10 +639,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -656,7 +653,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -671,8 +668,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
+      <c r="A10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
@@ -682,19 +679,19 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
+      <c r="A11" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
+      <c r="A12" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -711,12 +708,12 @@
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>13</v>
+      <c r="A14" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
@@ -755,19 +752,13 @@
         <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A18" s="5"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
@@ -820,14 +811,9 @@
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>